<commit_message>
feat : fixed length 구성
</commit_message>
<xml_diff>
--- a/src/main/resources/lottecard/template/commonHeader.xlsx
+++ b/src/main/resources/lottecard/template/commonHeader.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c697c9294f3e059c/바탕 화면/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{EE21E8A9-980E-4304-8113-9CB44A11A178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B252D06-FB19-4744-B695-D60DAA6C0720}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{EE21E8A9-980E-4304-8113-9CB44A11A178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91221FB2-49EF-4A4E-8A03-3494483A900D}"/>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="4020" windowWidth="29330" windowHeight="15580" xr2:uid="{0D6271A1-C031-425A-8197-9CD66A03B863}"/>
+    <workbookView xWindow="1300" yWindow="5730" windowWidth="29010" windowHeight="13880" xr2:uid="{0D6271A1-C031-425A-8197-9CD66A03B863}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,18 +36,148 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Field Name</t>
-  </si>
-  <si>
-    <t>Field Length</t>
-  </si>
-  <si>
-    <t>userId</t>
-  </si>
-  <si>
-    <t>userName</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+  <si>
+    <t>전문길이</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GUID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전문진행번호</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전문번호</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>요청응답구분</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TARGET 업무구분 코드</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전문요청일시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IP주소</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TARGET 서비스 ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>거래고유번호1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>거래고유번호2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>원거래 보장내용</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>시뮬레이션 거래여부</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전문응답일시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>처리결과코드</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>메시지응답코드</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>채널헤더 존재여부</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>여분필드</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fieldId</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fieldName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>length</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>offset</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>gramLnth</t>
+  </si>
+  <si>
+    <t>guid</t>
+  </si>
+  <si>
+    <t>gramPrgNo</t>
+  </si>
+  <si>
+    <t>gramNo</t>
+  </si>
+  <si>
+    <t>akRspDc</t>
+  </si>
+  <si>
+    <t>rspBizDc</t>
+  </si>
+  <si>
+    <t>gramAkDtti</t>
+  </si>
+  <si>
+    <t>ipAdd</t>
+  </si>
+  <si>
+    <t>tgtSvId</t>
+  </si>
+  <si>
+    <t>deNatvNo1</t>
+  </si>
+  <si>
+    <t>deNatvNo2</t>
+  </si>
+  <si>
+    <t>oriGrnCn</t>
+  </si>
+  <si>
+    <t>smlDeYn</t>
+  </si>
+  <si>
+    <t>gramRspDtti</t>
+  </si>
+  <si>
+    <t>pcRc</t>
+  </si>
+  <si>
+    <t>fstErrSysDc</t>
+  </si>
+  <si>
+    <t>chnlHdExsYn</t>
+  </si>
+  <si>
+    <t>exrFld</t>
   </si>
 </sst>
 </file>
@@ -80,20 +210,41 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -102,15 +253,18 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -446,40 +600,301 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCC6317A-2FE3-496B-884A-4D0FD1F20904}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.4140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
+      <c r="C3" s="1">
+        <v>31</v>
+      </c>
+      <c r="D3" s="1">
+        <f>C2+D2</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" ref="D4:D19" si="0">C3+D3</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="C12" s="1">
+        <v>9</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1">
+        <v>20</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1">
+        <v>17</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="C17" s="1">
+        <v>8</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="1">
+        <v>40</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>